<commit_message>
Successful simulation of blinking and adder configurations on 1x1 eFPGA (def did not forget to commit everything since init until now)
</commit_message>
<xml_diff>
--- a/eFPGA Memory Sizes.xlsx
+++ b/eFPGA Memory Sizes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13561f3231cadc0a/DTU/Research_Topics_in_Computer_Architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13561f3231cadc0a/DTU/Comp_Arch_2/eFPGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{5CDDF4ED-CFF6-4896-8902-F3B11B76877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{650F893B-DD0C-475B-A750-FBE2A1B41C7F}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{5CDDF4ED-CFF6-4896-8902-F3B11B76877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB51DCD-E65F-40DA-8C69-BC7837FF5D72}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{55F2CDF7-820B-407F-947D-0D6AA8888A49}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Add</t>
   </si>
   <si>
-    <t>2x2 eFPGA</t>
-  </si>
-  <si>
     <t>Memory Bits</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Choose between 0-3 synchronization registers, or for the signal chosen as clock 0-3 divisions</t>
+  </si>
+  <si>
+    <t>2x3 eFPGA</t>
   </si>
 </sst>
 </file>
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE99E594-1A45-4FC9-9FEB-756CEE2DE8B7}">
-  <dimension ref="B2:R18"/>
+  <dimension ref="B2:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,7 +502,7 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
@@ -553,7 +553,7 @@
         <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
@@ -593,7 +593,7 @@
         <v>32</v>
       </c>
       <c r="R4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
@@ -621,7 +621,7 @@
         <v>32</v>
       </c>
       <c r="R5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
@@ -663,7 +663,7 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f>C4</f>
@@ -731,7 +731,7 @@
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <f>32*7</f>
@@ -740,7 +740,7 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <f>D8+D11/32</f>
@@ -753,7 +753,7 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3">
         <f>C9*2+D12</f>
@@ -770,7 +770,7 @@
         <v>60320</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.35">
@@ -881,6 +881,16 @@
       <c r="L18">
         <f>16*32</f>
         <v>512</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <f>10*4</f>
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <f>10*4</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>